<commit_message>
Fixes for industry and commerce
Industry - upper shares. PLUS added growth constraint for industry other techs of HFO, ELC and GAS - these were jumping up too fast

Commerce - upper limits of shares for new other so that we dont have HFO running laptops.
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-PP.xlsx
+++ b/vt_REGION1_IND-PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA59659-D9E0-4F6E-AC22-A04C45EE2BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20BF75A-B55D-474C-BFC3-B42D958F8B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="742" firstSheet="19" activeTab="25" xr2:uid="{EADC4856-49BE-4DD1-AE06-BDD1A06F7643}"/>
   </bookViews>
@@ -58610,7 +58610,7 @@
   <dimension ref="A1:BE72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AW64" sqref="AW64"/>
+      <selection activeCell="AA60" sqref="AA60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed P&P PRC_RESID on new techs
This was causing veda to add NCAP_BND of zero to the techs and we were getting backstop.
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-PP.xlsx
+++ b/vt_REGION1_IND-PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B240B1ED-DD32-4997-B2F9-9FD4AB37328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0489D109-AC93-4EDA-A5C7-05C1DBDAB256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="742" firstSheet="13" activeTab="25" xr2:uid="{EADC4856-49BE-4DD1-AE06-BDD1A06F7643}"/>
   </bookViews>
@@ -6235,6 +6235,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -58731,8 +58732,8 @@
   </sheetPr>
   <dimension ref="A1:BE72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60965,9 +60966,7 @@
         <f>'ITEMS_Comm_BASE_JM '!B15</f>
         <v>IPPREC</v>
       </c>
-      <c r="H43" s="129">
-        <v>0</v>
-      </c>
+      <c r="H43" s="129"/>
       <c r="I43" s="129"/>
       <c r="N43" s="2"/>
       <c r="S43" s="120"/>
@@ -61079,9 +61078,7 @@
         <f>'ITEMS_Comm_BASE_JM '!B9</f>
         <v>IPPELC</v>
       </c>
-      <c r="H47" s="129">
-        <v>0</v>
-      </c>
+      <c r="H47" s="129"/>
       <c r="I47" s="129"/>
       <c r="N47" s="2"/>
       <c r="T47" s="129"/>
@@ -61213,9 +61210,7 @@
         <f>'ITEMS_Comm_BASE_JM '!B9</f>
         <v>IPPELC</v>
       </c>
-      <c r="H52" s="129">
-        <v>0</v>
-      </c>
+      <c r="H52" s="129"/>
       <c r="I52" s="129"/>
       <c r="N52" s="2"/>
       <c r="T52" s="129"/>
@@ -61348,9 +61343,7 @@
         <f>'ITEMS_Comm_BASE_JM '!B9</f>
         <v>IPPELC</v>
       </c>
-      <c r="H57" s="129">
-        <v>0</v>
-      </c>
+      <c r="H57" s="129"/>
       <c r="I57" s="129"/>
       <c r="N57" s="2"/>
       <c r="P57" s="120">
@@ -61447,9 +61440,7 @@
         <f>G31</f>
         <v>0.33025099075297226</v>
       </c>
-      <c r="H60" s="129">
-        <v>0</v>
-      </c>
+      <c r="H60" s="129"/>
       <c r="I60" s="129"/>
       <c r="N60" s="2"/>
       <c r="O60">
@@ -61517,9 +61508,7 @@
         <f>G32</f>
         <v>0.55391979116996026</v>
       </c>
-      <c r="H61" s="129">
-        <v>0</v>
-      </c>
+      <c r="H61" s="129"/>
       <c r="I61" s="129"/>
       <c r="N61" s="2"/>
       <c r="O61">
@@ -61587,9 +61576,7 @@
         <f>G33</f>
         <v>0.60401065424431821</v>
       </c>
-      <c r="H62" s="129">
-        <v>0</v>
-      </c>
+      <c r="H62" s="129"/>
       <c r="I62" s="129"/>
       <c r="N62" s="2"/>
       <c r="O62">
@@ -61645,9 +61632,7 @@
         <f>G34</f>
         <v>0.65516342057274379</v>
       </c>
-      <c r="H63" s="129">
-        <v>0</v>
-      </c>
+      <c r="H63" s="129"/>
       <c r="I63" s="129"/>
       <c r="N63" s="2"/>
       <c r="O63">

</xml_diff>